<commit_message>
Full Framework - Almost done
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software Testing\Workspace_Maven\TrainerManagement\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707E0F6A-BCC2-4346-A9B9-21FA45658BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625EA54D-B93C-4499-9C9D-9581159F8121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>admin@gmail.com</t>
   </si>
@@ -37,13 +37,25 @@
   </si>
   <si>
     <t>Pass@123</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Trainer</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +67,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,10 +101,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -366,38 +387,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{2C5C6067-75C3-45E3-A2AC-4B858A425638}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{288E93A1-E125-4D7C-A48B-00B602DC1588}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{A01CE05A-8E1B-44AD-B4CF-E825DF3576D5}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{2C5C6067-75C3-45E3-A2AC-4B858A425638}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{288E93A1-E125-4D7C-A48B-00B602DC1588}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{A01CE05A-8E1B-44AD-B4CF-E825DF3576D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>